<commit_message>
Add original declaration, add revision ch2
</commit_message>
<xml_diff>
--- a/final-reports/report/tables_and_code/derivative-free-comparison.xlsx
+++ b/final-reports/report/tables_and_code/derivative-free-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catar\Projects\Research Projects\ThesisReport\MscThesis\final-reports\report\tables_and_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4B4C47-0A3B-4BF1-B5DD-E62AC1DAE80E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07E2DAE-3524-4FED-A4A1-528E747AFD97}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4545" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{81D96340-F6D8-4B07-8BE7-0F6B09547F31}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{81D96340-F6D8-4B07-8BE7-0F6B09547F31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Metaheuristic</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>(evals)</t>
+  </si>
+  <si>
+    <t>No*</t>
   </si>
 </sst>
 </file>
@@ -178,12 +181,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="CMU Concrete"/>
+      <name val="CMU Serif"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="CMU Concrete"/>
+      <name val="CMU Serif"/>
     </font>
   </fonts>
   <fills count="3">
@@ -309,9 +312,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -322,16 +331,10 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,14 +652,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489C0F82-ED8C-4A4B-B2AB-F35598AFE665}">
   <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="1.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
@@ -729,7 +732,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>8</v>
@@ -831,13 +834,13 @@
         <v>19</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -863,38 +866,38 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="21" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>